<commit_message>
added ppm to column headings, edited petrolog examples for fo2/QFM consistency
</commit_message>
<xml_diff>
--- a/docs/Examples/Intro_Example_Petrolog_FC/PetrologCalculations.xlsx
+++ b/docs/Examples/Intro_Example_Petrolog_FC/PetrologCalculations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Berkeley_NEW\PySulfSat\PySulfSat_Structure\docs\Examples\Intro_Example_Petrolog_FC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D21BD2-7A9D-4711-8B4A-E1347BC5E99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5662617-EBDF-42A2-B9C7-7854D1FA55A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15960" activeTab="2" xr2:uid="{0529BD8F-C88F-4E4E-8348-A2BAF1D1D7E9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10540" firstSheet="1" activeTab="2" xr2:uid="{0529BD8F-C88F-4E4E-8348-A2BAF1D1D7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Petrolog_Output_FRAC_Olv" sheetId="4" r:id="rId1"/>
@@ -2618,8 +2618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90920F11-4703-4152-8398-A8A0BA1D5B50}">
   <dimension ref="A2:B22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2739,8 +2739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572120C9-D3FD-4F41-979E-C1B6093D433B}">
   <dimension ref="A1:BG32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
-      <selection activeCell="BJ5" sqref="BJ5"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AR3" sqref="AR3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>